<commit_message>
updated versioning for protocols
</commit_message>
<xml_diff>
--- a/inst/panels/panels_COVAIL.xlsx
+++ b/inst/panels/panels_COVAIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgeor10\Box\COVAIL\COVAIL_Rochester23X075F\data_meta\panels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\packages\COVAILworkflow\inst\panels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FE1282-33CA-4A6C-A5C2-CCF3E9830A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3191BCF-2B61-4C1F-8264-A41DE1FC0D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1935" yWindow="1230" windowWidth="38640" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3915" yWindow="2895" windowWidth="41895" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="panel_master" sheetId="1" r:id="rId1"/>
@@ -1440,7 +1440,7 @@
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,7 +2142,7 @@
         <v>274</v>
       </c>
       <c r="R18">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S18" t="s">
         <v>23</v>

</xml_diff>